<commit_message>
allow reshaping of newest data; add newest WFJ counts from Nomis
</commit_message>
<xml_diff>
--- a/INPUT/Stata_output BRES2018_rev.xlsx
+++ b/INPUT/Stata_output BRES2018_rev.xlsx
@@ -29698,9 +29698,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7432F78A-6840-4679-B6E2-FA88BCB43C45}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DA650FE-2377-4E1B-B89D-23ECD57453CE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{387D4674-E8B8-4C56-A8B0-04867F831439}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{702214A6-75D1-4692-BFD0-862CECD29A80}"/>
 </file>
</xml_diff>